<commit_message>
Further main menu & dialogue improvements
More animations
Settings menu
"Audio" tab of settings + Volume slider
Implemented automated main menu BG cycling
Made the black cover of the main menu wobble slightly at the edges

Some more test dialogue resources
Generalised dialogue option action

Folder rearrangement
Couple more translations
</commit_message>
<xml_diff>
--- a/External/Localisation.xlsx
+++ b/External/Localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riany\GODOT Projects\Roche-Limit\External\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B620849-9496-43E9-A858-0FE5FBFC9547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E301B1B-A4EE-4214-9F88-5F968D8871C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{A987F9A5-3EA6-40B1-A4F2-4DC9F39CDEEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
   <si>
     <t>key</t>
   </si>
@@ -482,9 +482,6 @@
     <t>IZAĆI</t>
   </si>
   <si>
-    <t>DIALOGUE_test/conv1/1</t>
-  </si>
-  <si>
     <t>This is a test dialogue string</t>
   </si>
   <si>
@@ -500,57 +497,12 @@
     <t>SETTINGS_accessibility</t>
   </si>
   <si>
-    <t>Audio</t>
-  </si>
-  <si>
     <t>SETTINGS_audio.master</t>
   </si>
   <si>
-    <t>Master</t>
-  </si>
-  <si>
     <t>SETTINGS_audio.music</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>SETTINGS_audio.sfx</t>
-  </si>
-  <si>
-    <t>SFX</t>
-  </si>
-  <si>
-    <t>SETTINGS_audio.players</t>
-  </si>
-  <si>
-    <t>Players</t>
-  </si>
-  <si>
-    <t>SETTINGS_audio.input</t>
-  </si>
-  <si>
-    <t>Input Device</t>
-  </si>
-  <si>
-    <t>SETTINGS_audio.input.vol</t>
-  </si>
-  <si>
-    <t>Input Volume</t>
-  </si>
-  <si>
-    <t>SETTINGS_audio.input.ptt</t>
-  </si>
-  <si>
-    <t>Push to Talk</t>
-  </si>
-  <si>
-    <t>SETTINGS_audio.input.open</t>
-  </si>
-  <si>
-    <t>Open Mic</t>
-  </si>
-  <si>
     <t>SETTINGS_audio.output</t>
   </si>
   <si>
@@ -567,6 +519,45 @@
   </si>
   <si>
     <t>Applies a low-pass filter to all audio to reduce high pitched noises</t>
+  </si>
+  <si>
+    <t>DIALOGUE_test/conv1/d1</t>
+  </si>
+  <si>
+    <t>DIALOGUE_test/conv1/d2</t>
+  </si>
+  <si>
+    <t>What the freak</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>SETTINGS_audio.menu_sfx</t>
+  </si>
+  <si>
+    <t>SETTINGS_audio.game_sfx</t>
+  </si>
+  <si>
+    <t>Game SFX Volume</t>
+  </si>
+  <si>
+    <t>Menu SFX Volume</t>
+  </si>
+  <si>
+    <t>Music Volume</t>
+  </si>
+  <si>
+    <t>Master Volume</t>
+  </si>
+  <si>
+    <t>Audio Settings</t>
   </si>
 </sst>
 </file>
@@ -960,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F89BA5F-BC43-4C0B-A0FC-3B29B9A1574C}">
-  <dimension ref="A1:AC29"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1508,121 +1499,106 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>149</v>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>